<commit_message>
Add info about Uzair to First Text_File.txt
</commit_message>
<xml_diff>
--- a/Acounts Section Data.xlsx
+++ b/Acounts Section Data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Admin\Desktop\Git Practice\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F72B7886-592C-437A-A564-2687C8941006}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ACC09773-6702-4160-8449-4CB147500959}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,9 +25,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1" uniqueCount="1">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
   <si>
     <t>Khizar Ahmad is a Good Boy</t>
+  </si>
+  <si>
+    <t>Uzair is More brilliant than Khizar</t>
   </si>
 </sst>
 </file>
@@ -345,9 +348,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:A2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
@@ -356,6 +361,11 @@
         <v>0</v>
       </c>
     </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>1</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>